<commit_message>
Add: Update Making Encrypt Key
</commit_message>
<xml_diff>
--- a/커뮤니티 프로젝트 설계서.xlsx
+++ b/커뮤니티 프로젝트 설계서.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\505-07\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\sif\Community_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="68">
   <si>
     <t>메뉴</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -181,6 +181,58 @@
   </si>
   <si>
     <t>유저, 관리자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jQuery를 이용해 ID/비밀번호 찾기 페이지로 이동</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jQuery를 이용해 회원가입 페이지로 이동</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ID/PW 찾기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Email 입력</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Email</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로그인 버튼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원가입 버튼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>따로 받은 생년, 생월, 생일을 조합해서 VO에 저장 후 DB에 INSERT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>링크 클릭 시 권한 업데이트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>메일로 발송된 인증링크</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DB 권한 테이블에서 아이디 권한 ROLE_USER로 업데이트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>유저 ID 값</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ajax를 이용해 해당 email로 가입된 아이디 체크, 아이디 첫 2글자 뒤에 **를 붙여서 보여줌</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -189,23 +241,31 @@
 2. Spring Security에서 지정해준 AuthenticationProvider를 상속받은 서비스로 login 정보 넘어감
 3. Provider에서 인증정보 ID를 기준으로 DB에서 정보 가져온 뒤 입력받은 비밀번호를 bCryptPasswordEncoder를 이용해 일치하는지 확인
 4. 일치하지 않으면 throw new SpringSecurityException, view에서 내용 보여줌
-5. 일치하면 유저정보와 권한이 담긴 토큰 return. 이 리턴된 토큰은 SecurityContextHolder에 저장됨.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>jQuery를 이용해 ID/비밀번호 찾기 페이지로 이동</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>jQuery를 이용해 회원가입 페이지로 이동</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ID/PW 찾기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ID찾기</t>
+5. 일치하면 유저정보와 권한이 담긴 토큰 return. 이 리턴된 토큰은 SecurityContextHolder에 저장됨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ID 찾기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>비밀번호 찾기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ID 입력</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이메일 형식 유효성 검사</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아이디 유효성 검사</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -213,51 +273,39 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Email</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ID찾기 버튼</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>로그인 버튼</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>회원가입 버튼</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>따로 받은 생년, 생월, 생일을 조합해서 VO에 저장 후 DB에 INSERT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>유효성 검사 통과 시 ajax를 이용해 form submit, 인증메일 발송, 권한 ROLE_UNAUTH로 저장</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>링크 클릭 시 권한 업데이트</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>메일로 발송된 인증링크</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DB 권한 테이블에서 아이디 권한 ROLE_USER로 업데이트</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ID찾기 버튼</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Email 값</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>유저 ID 값</t>
+    <t>비밀번호 찾기 버튼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ID 찾기 버튼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ID 찾기 버튼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>비밀번호 찾기 버튼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서버 과부하 방지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ajax를 이용해 form submit, 인증메일 발송, 권한 ROLE_UNAUTH로 저장</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>유효성 검사 통과 시 이메일 스팸 및 서버 부하를 줄이기 위해 ajax 완료될 때까지 버튼 기능 끄기
+ajax 완료 후 버튼 기능 켜기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ajax를 이용해 아이디와 이메일 값 체크
+1. 등록되지 않은 아이디, 등록된 아이디지만 email이 다름, 등록된 ID와 email이 같은 경우, 메일발송 실패
+4가지 경우로 나누어 사용자에게 알림
+2. 등록된 ID와 email이 같은 경우만 ID 입력, Email 입력창 value 지움</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -647,10 +695,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -658,9 +706,9 @@
     <col min="1" max="1" width="12.125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.5" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="93.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="100.125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="32.875" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" width="9" style="1"/>
@@ -703,130 +751,126 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="33" x14ac:dyDescent="0.3">
       <c r="A3" s="6"/>
-      <c r="B3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>20</v>
+        <v>64</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="6"/>
-      <c r="B4" s="5"/>
+      <c r="B4" s="5" t="s">
+        <v>4</v>
+      </c>
       <c r="C4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>32</v>
+        <v>5</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
+      <c r="B5" s="5"/>
       <c r="C5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="6"/>
       <c r="B6" s="6"/>
       <c r="C6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="6"/>
       <c r="B7" s="6"/>
       <c r="C7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="C8" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="33" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
-      <c r="D10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="33" x14ac:dyDescent="0.3">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="D11" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>34</v>
+        <v>12</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="D12" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>34</v>
@@ -835,118 +879,169 @@
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
-      <c r="C13" s="1" t="s">
-        <v>48</v>
+      <c r="D13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="6"/>
-      <c r="B14" s="7"/>
+      <c r="B14" s="6"/>
       <c r="C14" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="6"/>
-      <c r="B15" s="5" t="s">
-        <v>15</v>
-      </c>
+      <c r="B15" s="7"/>
       <c r="C15" s="1" t="s">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
+      <c r="B16" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="C16" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="115.5" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="115.5" x14ac:dyDescent="0.3">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="1" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="6"/>
-      <c r="B19" s="7"/>
+      <c r="B19" s="6"/>
       <c r="C19" s="1" t="s">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
-      <c r="B20" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="B20" s="7"/>
       <c r="C20" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>44</v>
+        <v>1</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>45</v>
+        <v>1</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="4"/>
+      <c r="B21" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="D21" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D22" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C23" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>46</v>
+      <c r="D23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D24" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="66" x14ac:dyDescent="0.3">
+      <c r="D25" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>